<commit_message>
[Soumya] Add: Sort And Send Email Template
</commit_message>
<xml_diff>
--- a/Contacts.xlsx
+++ b/Contacts.xlsx
@@ -31,9 +31,6 @@
     <t>West Bengal</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
     <t>Pranoy</t>
   </si>
   <si>
@@ -80,6 +77,9 @@
   </si>
   <si>
     <t>Email</t>
+  </si>
+  <si>
+    <t>soumyadipta0077@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,28 +447,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>15</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>18</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -494,21 +494,21 @@
         <v>9999999999</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
@@ -520,21 +520,21 @@
         <v>7777777777</v>
       </c>
       <c r="H3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>9</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -546,7 +546,7 @@
         <v>7776666666</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>